<commit_message>
metodos novos e a comparação
</commit_message>
<xml_diff>
--- a/Resultado dos métodos.xlsx
+++ b/Resultado dos métodos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programação\Quarentena_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B7000-7CBB-494C-9D4B-5A478D4AD136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE23146-1827-4F79-968F-15D9127278E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18165" yWindow="270" windowWidth="21600" windowHeight="11385" xr2:uid="{8863480A-3EF2-4630-B707-CFBA02486A1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8863480A-3EF2-4630-B707-CFBA02486A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Pontuação = 2475.91, Raiz = 49.76</t>
   </si>
@@ -145,13 +145,133 @@
   </si>
   <si>
     <t>SVR - Sigmoid:</t>
+  </si>
+  <si>
+    <t>NU_NOTA_CN</t>
+  </si>
+  <si>
+    <t>NU_NOTA_CH</t>
+  </si>
+  <si>
+    <t>NU_NOTA_MT</t>
+  </si>
+  <si>
+    <t>NU_NOTA_REDACAO</t>
+  </si>
+  <si>
+    <t>Estatística de regressão</t>
+  </si>
+  <si>
+    <t>R múltiplo</t>
+  </si>
+  <si>
+    <t>R-Quadrado</t>
+  </si>
+  <si>
+    <t>R-quadrado ajustado</t>
+  </si>
+  <si>
+    <t>Erro padrão</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regressão</t>
+  </si>
+  <si>
+    <t>Resíduo</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Interseção</t>
+  </si>
+  <si>
+    <t>gl</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F de significação</t>
+  </si>
+  <si>
+    <t>Coeficientes</t>
+  </si>
+  <si>
+    <t>Stat t</t>
+  </si>
+  <si>
+    <t>valor-P</t>
+  </si>
+  <si>
+    <t>95% inferiores</t>
+  </si>
+  <si>
+    <t>95% superiores</t>
+  </si>
+  <si>
+    <t>Inferior 95,0%</t>
+  </si>
+  <si>
+    <t>Superior 95,0%</t>
+  </si>
+  <si>
+    <t>Regressão Linear Multipla (do excel)</t>
+  </si>
+  <si>
+    <t>Regressão Excel</t>
+  </si>
+  <si>
+    <t>erro padrão = 46,32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLPRegressor: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pontuação = 2163.41, Raiz = 46.51</t>
+  </si>
+  <si>
+    <t>Neural network models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BayesianRidge: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2177.38, Raiz = 46.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasso </t>
+  </si>
+  <si>
+    <t>Pontuação = 2177.39, Raiz = 46.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNeighborsRegressor </t>
+  </si>
+  <si>
+    <t>Pontuação = 2455.09, Raiz = 49.55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +317,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +363,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -369,11 +526,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -419,12 +642,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -733,33 +1007,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB32F634-A00B-4A31-ADD8-FE73EBD4A6E7}">
-  <dimension ref="B1:Q37"/>
+  <dimension ref="B1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="47.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="2:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="22"/>
       <c r="E2" s="18"/>
       <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="2:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
+    </row>
+    <row r="3" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="20" t="s">
         <v>26</v>
       </c>
@@ -770,8 +1064,17 @@
         <v>28</v>
       </c>
       <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="30"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -781,8 +1084,19 @@
       <c r="E4" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="46"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -795,8 +1109,21 @@
       <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H5" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.76846255090506055</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -809,8 +1136,21 @@
       <c r="E6" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H6" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0.59053469214351284</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
@@ -823,17 +1163,40 @@
       <c r="E7" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H7" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0.59052377270465539</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="19"/>
       <c r="E8" s="12"/>
+      <c r="H8" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="48">
+        <v>46.319635815601103</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
@@ -844,185 +1207,701 @@
         <v>32</v>
       </c>
       <c r="E9" s="13"/>
+      <c r="H9" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="26">
+        <v>150000</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="13"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="13"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="13"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="19"/>
       <c r="E14" s="13"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="13"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="7"/>
-    </row>
-    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="13"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23" t="s">
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="13"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="13"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="13"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="13"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="13"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="13"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="13"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="13"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="E26" s="13"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="H29" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="37">
+        <v>4</v>
+      </c>
+      <c r="J29" s="37">
+        <v>464125423.95141804</v>
+      </c>
+      <c r="K29" s="37">
+        <v>116031355.98785451</v>
+      </c>
+      <c r="L29" s="37">
+        <v>54081.047556727011</v>
+      </c>
+      <c r="M29" s="35">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="13"/>
+      <c r="H30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="37">
+        <v>149995</v>
+      </c>
+      <c r="J30" s="37">
+        <v>321815571.77017701</v>
+      </c>
+      <c r="K30" s="37">
+        <v>2145.5086620899165</v>
+      </c>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="H31" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="38">
+        <v>149999</v>
+      </c>
+      <c r="J31" s="38">
+        <v>785940995.72159505</v>
+      </c>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="E32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="E17" s="12"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="C33" s="24"/>
+      <c r="E33" s="12"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="P33" s="34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="E34" s="12"/>
+      <c r="H34" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" s="37">
+        <v>128.56928353790531</v>
+      </c>
+      <c r="J34" s="37">
+        <v>0.9828090577186267</v>
+      </c>
+      <c r="K34" s="37">
+        <v>130.81817116780587</v>
+      </c>
+      <c r="L34" s="35">
+        <v>0</v>
+      </c>
+      <c r="M34" s="37">
+        <v>126.64299763719087</v>
+      </c>
+      <c r="N34" s="37">
+        <v>130.49556943861973</v>
+      </c>
+      <c r="O34" s="37">
+        <v>126.64299763719087</v>
+      </c>
+      <c r="P34" s="39">
+        <v>130.49556943861973</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="E35" s="12"/>
+      <c r="H35" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="37">
+        <v>0.16346408936376738</v>
+      </c>
+      <c r="J35" s="37">
+        <v>2.1954770637893925E-3</v>
+      </c>
+      <c r="K35" s="37">
+        <v>74.454929208701657</v>
+      </c>
+      <c r="L35" s="35">
+        <v>0</v>
+      </c>
+      <c r="M35" s="37">
+        <v>0.15916099866664218</v>
+      </c>
+      <c r="N35" s="37">
+        <v>0.16776718006089258</v>
+      </c>
+      <c r="O35" s="37">
+        <v>0.15916099866664218</v>
+      </c>
+      <c r="P35" s="39">
+        <v>0.16776718006089258</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="E36" s="12"/>
+      <c r="H36" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" s="37">
+        <v>0.39569749521896291</v>
+      </c>
+      <c r="J36" s="37">
+        <v>1.9800809037224618E-3</v>
+      </c>
+      <c r="K36" s="41">
+        <v>199.83905429069574</v>
+      </c>
+      <c r="L36" s="35">
+        <v>0</v>
+      </c>
+      <c r="M36" s="37">
+        <v>0.39181657664463854</v>
+      </c>
+      <c r="N36" s="37">
+        <v>0.39957841379328729</v>
+      </c>
+      <c r="O36" s="37">
+        <v>0.39181657664463854</v>
+      </c>
+      <c r="P36" s="39">
+        <v>0.39957841379328729</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
+      <c r="E37" s="12"/>
+      <c r="H37" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="37">
+        <v>0.10626034335000274</v>
+      </c>
+      <c r="J37" s="37">
+        <v>1.5257197920507358E-3</v>
+      </c>
+      <c r="K37" s="37">
+        <v>69.646041103771168</v>
+      </c>
+      <c r="L37" s="35">
+        <v>0</v>
+      </c>
+      <c r="M37" s="37">
+        <v>0.10326996337661254</v>
+      </c>
+      <c r="N37" s="37">
+        <v>0.10925072332339295</v>
+      </c>
+      <c r="O37" s="37">
+        <v>0.10326996337661254</v>
+      </c>
+      <c r="P37" s="39">
+        <v>0.10925072332339295</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="E38" s="12"/>
+      <c r="H38" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I38" s="38">
+        <v>7.0630497395339442E-2</v>
+      </c>
+      <c r="J38" s="38">
+        <v>8.1077714512186835E-4</v>
+      </c>
+      <c r="K38" s="38">
+        <v>87.114563872817271</v>
+      </c>
+      <c r="L38" s="51">
+        <v>0</v>
+      </c>
+      <c r="M38" s="38">
+        <v>6.9041390568327587E-2</v>
+      </c>
+      <c r="N38" s="38">
+        <v>7.2219604222351297E-2</v>
+      </c>
+      <c r="O38" s="38">
+        <v>6.9041390568327587E-2</v>
+      </c>
+      <c r="P38" s="40">
+        <v>7.2219604222351297E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="4"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="E42" s="12"/>
+      <c r="J42" s="36"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="E45" s="14"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Testes de parametros do MLP
</commit_message>
<xml_diff>
--- a/Resultado dos métodos.xlsx
+++ b/Resultado dos métodos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programação\Quarentena_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE23146-1827-4F79-968F-15D9127278E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137AF45-96EE-4D00-AD03-C6B2A27B52BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8863480A-3EF2-4630-B707-CFBA02486A1D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
   <si>
     <t>Pontuação = 2475.91, Raiz = 49.76</t>
   </si>
@@ -265,13 +265,94 @@
   </si>
   <si>
     <t>Pontuação = 2455.09, Raiz = 49.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLPRegressor </t>
+  </si>
+  <si>
+    <t>Pontuação = 2089.16, Raiz = 45.71</t>
+  </si>
+  <si>
+    <t>Pontuação = 2177.25, Raiz = 46.66</t>
+  </si>
+  <si>
+    <t>Pontuação = 2177.24, Raiz = 46.66</t>
+  </si>
+  <si>
+    <t>Juntando todas as notas</t>
+  </si>
+  <si>
+    <t>Pontuação = 2318.55, Raiz = 48.15</t>
+  </si>
+  <si>
+    <t>Pontuação = 2220.09, Raiz = 47.12</t>
+  </si>
+  <si>
+    <t>Pontuação = 2154.20, Raiz = 46.41</t>
+  </si>
+  <si>
+    <t>Pontuação = 2094.61, Raiz = 45.77</t>
+  </si>
+  <si>
+    <t>Pontuação = 2277.50, Raiz = 47.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP alpha=0.00001: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2130.73, Raiz = 46.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP alpha=0.001: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2182.35, Raiz = 46.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP alpha=0.01: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2090.12, Raiz = 45.72</t>
+  </si>
+  <si>
+    <t>Pontuação = 2088.25, Raiz = 45.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP alpha=1: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP alpha=3: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2137.77, Raiz = 46.24</t>
+  </si>
+  <si>
+    <t>Testando configurações do MLPRegressor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver = lbfgs: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver = adam: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activation = identity: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activation = logistic: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activation = tanh: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activation = relu: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +435,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -596,14 +684,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -617,7 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,18 +715,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -665,6 +739,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,14 +774,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB32F634-A00B-4A31-ADD8-FE73EBD4A6E7}">
-  <dimension ref="B1:P53"/>
+  <dimension ref="B1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,48 +1126,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="15"/>
-      <c r="H2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="44"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="48"/>
     </row>
     <row r="3" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="30"/>
+      <c r="F3" s="13"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1081,19 +1176,19 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -1103,24 +1198,24 @@
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="19">
         <v>0.76846255090506055</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -1130,24 +1225,24 @@
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="19">
         <v>0.59053469214351284</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -1157,751 +1252,904 @@
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="19">
         <v>0.59052377270465539</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="12"/>
-      <c r="H8" s="47" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="11"/>
+      <c r="H8" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="37">
         <v>46.319635815601103</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="H9" s="32" t="s">
+      <c r="E9" s="12"/>
+      <c r="H9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="20">
         <v>150000</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="13"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="12"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="13"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="12"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="13"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="12"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="13"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="12"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="13"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="12"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="13"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="12"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="13"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="13"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="12"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="13"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="30"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="13"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="12"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="13"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="12"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="13"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="56"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
+      <c r="B22" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="6"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="13"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="55"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="13"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="55"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="13"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
+    <row r="25" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="55"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="13"/>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="55"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E27" s="6"/>
       <c r="H27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="55"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="27" t="s">
+      <c r="J28" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="L28" s="27" t="s">
+      <c r="L28" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="M28" s="27" t="s">
+      <c r="M28" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="H29" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="55"/>
+      <c r="H29" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I29" s="37">
+      <c r="I29" s="31">
         <v>4</v>
       </c>
-      <c r="J29" s="37">
+      <c r="J29" s="31">
         <v>464125423.95141804</v>
       </c>
-      <c r="K29" s="37">
+      <c r="K29" s="31">
         <v>116031355.98785451</v>
       </c>
-      <c r="L29" s="37">
+      <c r="L29" s="31">
         <v>54081.047556727011</v>
       </c>
-      <c r="M29" s="35">
+      <c r="M29" s="29">
         <v>0</v>
       </c>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
-      <c r="E30" s="13"/>
-      <c r="H30" s="31" t="s">
+      <c r="E30" s="55"/>
+      <c r="H30" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="37">
+      <c r="I30" s="31">
         <v>149995</v>
       </c>
-      <c r="J30" s="37">
+      <c r="J30" s="31">
         <v>321815571.77017701</v>
       </c>
-      <c r="K30" s="37">
+      <c r="K30" s="31">
         <v>2145.5086620899165</v>
       </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="H31" s="32" t="s">
+    <row r="31" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="E31" s="55"/>
+      <c r="H31" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="38">
+      <c r="I31" s="32">
         <v>149999</v>
       </c>
-      <c r="J31" s="38">
+      <c r="J31" s="32">
         <v>785940995.72159505</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="6"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="E33" s="12"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="27" t="s">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J33" s="27" t="s">
+      <c r="J33" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K33" s="27" t="s">
+      <c r="K33" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="27" t="s">
+      <c r="L33" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="M33" s="27" t="s">
+      <c r="M33" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="N33" s="27" t="s">
+      <c r="N33" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="O33" s="27" t="s">
+      <c r="O33" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="P33" s="34" t="s">
+      <c r="P33" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="H34" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="H34" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I34" s="37">
+      <c r="I34" s="31">
         <v>128.56928353790531</v>
       </c>
-      <c r="J34" s="37">
+      <c r="J34" s="31">
         <v>0.9828090577186267</v>
       </c>
-      <c r="K34" s="37">
+      <c r="K34" s="31">
         <v>130.81817116780587</v>
       </c>
-      <c r="L34" s="35">
+      <c r="L34" s="29">
         <v>0</v>
       </c>
-      <c r="M34" s="37">
+      <c r="M34" s="31">
         <v>126.64299763719087</v>
       </c>
-      <c r="N34" s="37">
+      <c r="N34" s="31">
         <v>130.49556943861973</v>
       </c>
-      <c r="O34" s="37">
+      <c r="O34" s="31">
         <v>126.64299763719087</v>
       </c>
-      <c r="P34" s="39">
+      <c r="P34" s="33">
         <v>130.49556943861973</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="H35" s="31" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="E35" s="6"/>
+      <c r="H35" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="37">
+      <c r="I35" s="31">
         <v>0.16346408936376738</v>
       </c>
-      <c r="J35" s="37">
+      <c r="J35" s="31">
         <v>2.1954770637893925E-3</v>
       </c>
-      <c r="K35" s="37">
+      <c r="K35" s="31">
         <v>74.454929208701657</v>
       </c>
-      <c r="L35" s="35">
+      <c r="L35" s="29">
         <v>0</v>
       </c>
-      <c r="M35" s="37">
+      <c r="M35" s="31">
         <v>0.15916099866664218</v>
       </c>
-      <c r="N35" s="37">
+      <c r="N35" s="31">
         <v>0.16776718006089258</v>
       </c>
-      <c r="O35" s="37">
+      <c r="O35" s="31">
         <v>0.15916099866664218</v>
       </c>
-      <c r="P35" s="39">
+      <c r="P35" s="33">
         <v>0.16776718006089258</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="H36" s="31" t="s">
+    <row r="36" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="E36" s="6"/>
+      <c r="H36" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="37">
+      <c r="I36" s="31">
         <v>0.39569749521896291</v>
       </c>
-      <c r="J36" s="37">
+      <c r="J36" s="31">
         <v>1.9800809037224618E-3</v>
       </c>
-      <c r="K36" s="41">
+      <c r="K36" s="35">
         <v>199.83905429069574</v>
       </c>
-      <c r="L36" s="35">
+      <c r="L36" s="29">
         <v>0</v>
       </c>
-      <c r="M36" s="37">
+      <c r="M36" s="31">
         <v>0.39181657664463854</v>
       </c>
-      <c r="N36" s="37">
+      <c r="N36" s="31">
         <v>0.39957841379328729</v>
       </c>
-      <c r="O36" s="37">
+      <c r="O36" s="31">
         <v>0.39181657664463854</v>
       </c>
-      <c r="P36" s="39">
+      <c r="P36" s="33">
         <v>0.39957841379328729</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="H37" s="31" t="s">
+    <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="45"/>
+      <c r="E37" s="6"/>
+      <c r="H37" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I37" s="37">
+      <c r="I37" s="31">
         <v>0.10626034335000274</v>
       </c>
-      <c r="J37" s="37">
+      <c r="J37" s="31">
         <v>1.5257197920507358E-3</v>
       </c>
-      <c r="K37" s="37">
+      <c r="K37" s="31">
         <v>69.646041103771168</v>
       </c>
-      <c r="L37" s="35">
+      <c r="L37" s="29">
         <v>0</v>
       </c>
-      <c r="M37" s="37">
+      <c r="M37" s="31">
         <v>0.10326996337661254</v>
       </c>
-      <c r="N37" s="37">
+      <c r="N37" s="31">
         <v>0.10925072332339295</v>
       </c>
-      <c r="O37" s="37">
+      <c r="O37" s="31">
         <v>0.10326996337661254</v>
       </c>
-      <c r="P37" s="39">
+      <c r="P37" s="33">
         <v>0.10925072332339295</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="E38" s="12"/>
-      <c r="H38" s="32" t="s">
+      <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="H38" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="32">
         <v>7.0630497395339442E-2</v>
       </c>
-      <c r="J38" s="38">
+      <c r="J38" s="32">
         <v>8.1077714512186835E-4</v>
       </c>
-      <c r="K38" s="38">
+      <c r="K38" s="32">
         <v>87.114563872817271</v>
       </c>
-      <c r="L38" s="51">
+      <c r="L38" s="40">
         <v>0</v>
       </c>
-      <c r="M38" s="38">
+      <c r="M38" s="32">
         <v>6.9041390568327587E-2</v>
       </c>
-      <c r="N38" s="38">
+      <c r="N38" s="32">
         <v>7.2219604222351297E-2</v>
       </c>
-      <c r="O38" s="38">
+      <c r="O38" s="32">
         <v>6.9041390568327587E-2</v>
       </c>
-      <c r="P38" s="40">
+      <c r="P38" s="34">
         <v>7.2219604222351297E-2</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="E39" s="12"/>
+      <c r="B39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="4"/>
-      <c r="E40" s="12"/>
+      <c r="B40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
-      <c r="E41" s="12"/>
+      <c r="B41" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
-      <c r="E42" s="12"/>
-      <c r="J42" s="36"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="E43" s="12"/>
+      <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="E45" s="14"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
-      <c r="C52" s="8"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="B44" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="J49" s="30"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="E51" s="55"/>
+    </row>
+    <row r="52" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="6"/>
+      <c r="D60" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="H2:P2"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Resultado dos métodos.xlsx
</commit_message>
<xml_diff>
--- a/Resultado dos métodos.xlsx
+++ b/Resultado dos métodos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programação\Quarentena_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137AF45-96EE-4D00-AD03-C6B2A27B52BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D0B24-3769-496C-B19D-0E71D9D5294E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8863480A-3EF2-4630-B707-CFBA02486A1D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="108">
   <si>
     <t>Pontuação = 2475.91, Raiz = 49.76</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t xml:space="preserve">activation = relu: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NuSVR: </t>
+  </si>
+  <si>
+    <t>Pontuação = 2096.64, Raiz = 45.79</t>
+  </si>
+  <si>
+    <t>*17 min</t>
   </si>
 </sst>
 </file>
@@ -747,16 +756,25 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -774,15 +792,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,7 +1114,7 @@
   <dimension ref="B1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,23 +1139,23 @@
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="52"/>
       <c r="E2" s="16"/>
       <c r="F2" s="13"/>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="48"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="18" t="s">
@@ -1179,10 +1188,10 @@
       <c r="E4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="50"/>
+      <c r="I4" s="57"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1292,10 +1301,10 @@
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -1408,7 +1417,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="17"/>
       <c r="E15" s="12"/>
-      <c r="H15" s="57"/>
+      <c r="H15" s="48"/>
       <c r="I15" s="19"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1518,7 +1527,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="56"/>
+      <c r="E21" s="47"/>
       <c r="H21" s="25"/>
       <c r="I21" s="19"/>
       <c r="J21" s="6"/>
@@ -1552,7 +1561,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="17"/>
-      <c r="E23" s="55"/>
+      <c r="E23" s="46"/>
       <c r="H23" s="25"/>
       <c r="I23" s="19"/>
       <c r="J23" s="6"/>
@@ -1567,7 +1576,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="55"/>
+      <c r="E24" s="46"/>
       <c r="H24" s="25"/>
       <c r="I24" s="19"/>
       <c r="J24" s="6"/>
@@ -1579,12 +1588,12 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="45"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="55"/>
+      <c r="E25" s="46"/>
       <c r="H25" s="25"/>
       <c r="I25" s="19"/>
       <c r="J25" s="6"/>
@@ -1602,7 +1611,7 @@
       <c r="C26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="55"/>
+      <c r="E26" s="46"/>
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -1640,7 +1649,7 @@
       <c r="C28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="55"/>
+      <c r="E28" s="46"/>
       <c r="H28" s="27"/>
       <c r="I28" s="21" t="s">
         <v>53</v>
@@ -1668,7 +1677,7 @@
       <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="55"/>
+      <c r="E29" s="46"/>
       <c r="H29" s="25" t="s">
         <v>49</v>
       </c>
@@ -1694,7 +1703,7 @@
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
-      <c r="E30" s="55"/>
+      <c r="E30" s="46"/>
       <c r="H30" s="25" t="s">
         <v>50</v>
       </c>
@@ -1714,11 +1723,11 @@
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="E31" s="55"/>
+      <c r="C31" s="50"/>
+      <c r="E31" s="46"/>
       <c r="H31" s="26" t="s">
         <v>51</v>
       </c>
@@ -1736,10 +1745,10 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C32" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E32" s="6"/>
@@ -1794,7 +1803,7 @@
       <c r="C34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="46"/>
       <c r="H34" s="25" t="s">
         <v>52</v>
       </c>
@@ -1824,8 +1833,15 @@
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>107</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="H35" s="25" t="s">
         <v>38</v>
@@ -1888,10 +1904,10 @@
       </c>
     </row>
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="45"/>
+      <c r="C37" s="50"/>
       <c r="E37" s="6"/>
       <c r="H37" s="25" t="s">
         <v>40</v>
@@ -1976,10 +1992,10 @@
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="53" t="s">
+      <c r="C41" s="44" t="s">
         <v>86</v>
       </c>
       <c r="E41" s="6"/>
@@ -1999,10 +2015,10 @@
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="53" t="s">
+      <c r="C44" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="6"/>
@@ -2013,7 +2029,7 @@
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="42" t="s">
         <v>88</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2040,10 +2056,10 @@
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="53" t="s">
+      <c r="C49" s="44" t="s">
         <v>94</v>
       </c>
       <c r="E49" s="6"/>
@@ -2061,7 +2077,7 @@
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
-      <c r="E51" s="55"/>
+      <c r="E51" s="46"/>
     </row>
     <row r="52" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>

</xml_diff>